<commit_message>
Started work on PCB Layout, still want to check if I2C onto the JST connector is possible/useful.
</commit_message>
<xml_diff>
--- a/BOM/BOM_ArmPowerBoard_V3.xlsx
+++ b/BOM/BOM_ArmPowerBoard_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{23C58643-9FA2-4726-A87F-F2219B46D548}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDBC16-3402-4271-803D-FD716D06CE1B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
   <si>
     <t>Description</t>
   </si>
@@ -144,18 +144,9 @@
     <t>Total of three</t>
   </si>
   <si>
-    <t>CONN HDR 11POS 0.1 TIN PCB</t>
-  </si>
-  <si>
-    <t>PPTC111LFBN-RC</t>
-  </si>
-  <si>
     <t>arduino GPIO</t>
   </si>
   <si>
-    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC111LFBN-RC/S7009-ND/810150</t>
-  </si>
-  <si>
     <t>https://www.digikey.com/products/en?keywords=9B-16.000MBBK-B</t>
   </si>
   <si>
@@ -174,21 +165,9 @@
     <t>B7B-PH-SM4-TB(LF)(SN)</t>
   </si>
   <si>
-    <t>serial port</t>
-  </si>
-  <si>
     <t>https://www.digikey.ca/product-detail/en/jst-sales-america-inc/B7B-PH-SM4-TB-LF-SN/455-1739-1-ND/926836</t>
   </si>
   <si>
-    <t>usb port</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/molex-llc/0483930003/WM10413CT-ND/4701505</t>
-  </si>
-  <si>
-    <t>CONN RCPT USB3.0 TYPEA 9POS R/A</t>
-  </si>
-  <si>
     <t>TERM BLK 4P SIDE ENT 5.08MM PCB</t>
   </si>
   <si>
@@ -201,12 +180,6 @@
     <t>https://www.digikey.ca/product-detail/en/weidm-ller/1330730000/281-4010-ND/5997483</t>
   </si>
   <si>
-    <t>zener Diode</t>
-  </si>
-  <si>
-    <t>Voltage regulating Capacitor</t>
-  </si>
-  <si>
     <t>SENSOR CURRENT HALL 100A AC/DC</t>
   </si>
   <si>
@@ -270,16 +243,115 @@
     <t>https://solarbotics.com/product/50222/</t>
   </si>
   <si>
-    <t>use this for 5v power?</t>
-  </si>
-  <si>
-    <t>We have 2 good ones</t>
-  </si>
-  <si>
-    <t>electrical</t>
-  </si>
-  <si>
-    <t>Arm PowerBoard</t>
+    <t>DIODE ZENER 28V 5W DO214AA</t>
+  </si>
+  <si>
+    <t>SMBJ5362B-TP</t>
+  </si>
+  <si>
+    <t>CAP ALUM 220UF 20% 25V SMD</t>
+  </si>
+  <si>
+    <t>AFK227M25F24T-F</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/cornell-dubilier-electronics-cde/AFK227M25F24T-F/338-2171-1-ND/2404234</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/micro-commercial-co/SMBJ5362B-TP/SMBJ5362B-TPMSCT-ND/1636228</t>
+  </si>
+  <si>
+    <t>15 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200, Moisture Resistant Thick Film</t>
+  </si>
+  <si>
+    <t>CRGCQ0402F15R</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/te-connectivity-passive-product/CRGCQ0402F15R/A129605CT-ND/8577437</t>
+  </si>
+  <si>
+    <t>15Ohm for zener Diode</t>
+  </si>
+  <si>
+    <t>min 12 Ohm current limiting</t>
+  </si>
+  <si>
+    <t>SparkFun USB to Serial Breakout </t>
+  </si>
+  <si>
+    <t>FT232RL</t>
+  </si>
+  <si>
+    <t>sparkfun</t>
+  </si>
+  <si>
+    <t>usb to serial</t>
+  </si>
+  <si>
+    <t>https://www.sparkfun.com/products/12731</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>We have unused 2 good ones</t>
+  </si>
+  <si>
+    <t>serial port 7 pin</t>
+  </si>
+  <si>
+    <t>(lots in random minirover stuff)</t>
+  </si>
+  <si>
+    <t>PPTC141LFBN-RC</t>
+  </si>
+  <si>
+    <t>CONN HDR 14POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC141LFBN-RC/S7012-ND/810152</t>
+  </si>
+  <si>
+    <t>CONN HEADER VERT 9POS 2.54MM</t>
+  </si>
+  <si>
+    <t>male</t>
+  </si>
+  <si>
+    <t>female</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/wurth-electronics-inc/61300911121/732-5322-ND/4846843</t>
+  </si>
+  <si>
+    <t>CONN HDR 9POS 0.1 TIN PCB</t>
+  </si>
+  <si>
+    <t>PPTC091LFBN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC091LFBN-RC/S7007-ND/810148</t>
+  </si>
+  <si>
+    <t>red Led</t>
+  </si>
+  <si>
+    <t>tons</t>
+  </si>
+  <si>
+    <t>CONN IC DIP SOCKET 28POS TIN</t>
+  </si>
+  <si>
+    <t>ED281DT</t>
+  </si>
+  <si>
+    <t>atmega holder</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/on-shore-technology-inc/ED281DT/ED3050-5-ND/4147600</t>
+  </si>
+  <si>
+    <t>ArmPowerBoard</t>
   </si>
 </sst>
 </file>
@@ -290,7 +362,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="15">
+  <fonts count="17">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -401,6 +473,20 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF555555"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="6">
     <fill>
@@ -462,7 +548,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -504,12 +590,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
@@ -525,6 +605,16 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="16" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -847,8 +937,8 @@
   </sheetPr>
   <dimension ref="B2:J63"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -865,10 +955,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="23.4">
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="20"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -885,7 +975,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>80</v>
+        <v>105</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -894,13 +984,11 @@
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="33">
-        <v>43491</v>
+      <c r="C5" s="31">
+        <v>43498</v>
       </c>
       <c r="D5" s="1"/>
-      <c r="E5" s="1" t="s">
-        <v>81</v>
-      </c>
+      <c r="E5" s="1"/>
     </row>
     <row r="6" spans="2:10" ht="21">
       <c r="B6" s="3"/>
@@ -914,7 +1002,7 @@
       </c>
       <c r="C7" s="10">
         <f>SUM(G11:G41)</f>
-        <v>198.32</v>
+        <v>296.56</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
@@ -993,14 +1081,14 @@
         <v>1</v>
       </c>
       <c r="F12" s="13">
-        <v>2.21</v>
+        <v>2.13</v>
       </c>
       <c r="G12" s="13">
-        <f t="shared" ref="G12:G39" si="0">E12*F12</f>
-        <v>2.21</v>
+        <f t="shared" ref="G12:G43" si="0">E12*F12</f>
+        <v>2.13</v>
       </c>
       <c r="H12" s="17" t="s">
-        <v>52</v>
+        <v>45</v>
       </c>
       <c r="I12" s="12"/>
       <c r="J12" s="15" t="s">
@@ -1009,7 +1097,7 @@
     </row>
     <row r="13" spans="2:10" ht="15.6">
       <c r="B13" s="12" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="C13" s="12">
         <v>1330730000</v>
@@ -1019,70 +1107,70 @@
         <v>1</v>
       </c>
       <c r="F13" s="13">
-        <v>3.78</v>
+        <v>3.63</v>
       </c>
       <c r="G13" s="13">
         <f t="shared" si="0"/>
-        <v>3.78</v>
+        <v>3.63</v>
       </c>
       <c r="H13" s="17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="I13" s="12"/>
-      <c r="J13" s="12" t="s">
-        <v>54</v>
+      <c r="J13" s="15" t="s">
+        <v>47</v>
       </c>
     </row>
     <row r="14" spans="2:10" ht="15.6">
       <c r="B14" s="12" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="C14" s="17" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="D14" s="12"/>
       <c r="E14" s="12">
         <v>3</v>
       </c>
       <c r="F14" s="13">
-        <v>1.03</v>
+        <v>0.99</v>
       </c>
       <c r="G14" s="13">
         <f t="shared" si="0"/>
-        <v>3.09</v>
+        <v>2.9699999999999998</v>
       </c>
       <c r="H14" s="17" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="I14" s="17"/>
       <c r="J14" s="15" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="2:10" ht="15.6">
       <c r="B15" s="12" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="C15" s="12" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="D15" s="12"/>
       <c r="E15" s="12">
         <v>2</v>
       </c>
       <c r="F15" s="13">
-        <v>1.0900000000000001</v>
+        <v>1.05</v>
       </c>
       <c r="G15" s="13">
         <f t="shared" si="0"/>
-        <v>2.1800000000000002</v>
+        <v>2.1</v>
       </c>
       <c r="H15" s="17" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="I15" s="12"/>
-      <c r="J15" s="12" t="s">
-        <v>67</v>
+      <c r="J15" s="15" t="s">
+        <v>58</v>
       </c>
     </row>
     <row r="16" spans="2:10" ht="15.6">
@@ -1090,25 +1178,25 @@
         <v>27</v>
       </c>
       <c r="C16" s="12" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="D16" s="12"/>
       <c r="E16" s="12">
         <v>1</v>
       </c>
       <c r="F16" s="13">
-        <v>1.18</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="G16" s="13">
         <f t="shared" si="0"/>
-        <v>1.18</v>
+        <v>1.1299999999999999</v>
       </c>
       <c r="H16" s="17" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="I16" s="12"/>
       <c r="J16" s="15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
     </row>
     <row r="17" spans="2:10" ht="15.6">
@@ -1162,7 +1250,9 @@
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H20" s="12"/>
+      <c r="H20" s="17" t="s">
+        <v>85</v>
+      </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
     </row>
@@ -1191,11 +1281,11 @@
         <v>1</v>
       </c>
       <c r="F22" s="13">
-        <v>173.57</v>
+        <v>246.07</v>
       </c>
       <c r="G22" s="13">
         <f t="shared" si="0"/>
-        <v>173.57</v>
+        <v>246.07</v>
       </c>
       <c r="H22" s="12"/>
       <c r="I22" s="12"/>
@@ -1205,74 +1295,104 @@
     </row>
     <row r="23" spans="2:10" ht="15.6">
       <c r="B23" s="17" t="s">
-        <v>55</v>
-      </c>
-      <c r="C23" s="12"/>
+        <v>69</v>
+      </c>
+      <c r="C23" s="17" t="s">
+        <v>70</v>
+      </c>
       <c r="D23" s="12"/>
-      <c r="E23" s="12"/>
-      <c r="F23" s="13"/>
+      <c r="E23" s="12">
+        <v>1</v>
+      </c>
+      <c r="F23" s="13">
+        <v>0.96</v>
+      </c>
       <c r="G23" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H23" s="12"/>
+        <v>0.96</v>
+      </c>
+      <c r="H23" s="17" t="s">
+        <v>79</v>
+      </c>
       <c r="I23" s="12"/>
-      <c r="J23" s="15"/>
+      <c r="J23" s="15" t="s">
+        <v>74</v>
+      </c>
     </row>
     <row r="24" spans="2:10" ht="15.6">
       <c r="B24" s="17" t="s">
-        <v>56</v>
-      </c>
-      <c r="C24" s="12"/>
+        <v>71</v>
+      </c>
+      <c r="C24" s="12" t="s">
+        <v>72</v>
+      </c>
       <c r="D24" s="12"/>
-      <c r="E24" s="12"/>
-      <c r="F24" s="13"/>
+      <c r="E24" s="12">
+        <v>1</v>
+      </c>
+      <c r="F24" s="13">
+        <v>1.72</v>
+      </c>
       <c r="G24" s="13">
         <f t="shared" si="0"/>
-        <v>0</v>
+        <v>1.72</v>
       </c>
       <c r="H24" s="12"/>
       <c r="I24" s="17"/>
-      <c r="J24" s="12"/>
+      <c r="J24" s="15" t="s">
+        <v>73</v>
+      </c>
     </row>
     <row r="25" spans="2:10" ht="15.6">
-      <c r="B25" s="30"/>
-      <c r="C25" s="30"/>
-      <c r="D25" s="30"/>
-      <c r="E25" s="30"/>
-      <c r="F25" s="31"/>
-      <c r="G25" s="31">
+      <c r="B25" s="28" t="s">
+        <v>75</v>
+      </c>
+      <c r="C25" s="21" t="s">
+        <v>76</v>
+      </c>
+      <c r="D25" s="28"/>
+      <c r="E25" s="28">
+        <v>10</v>
+      </c>
+      <c r="F25" s="29">
+        <v>3.5000000000000003E-2</v>
+      </c>
+      <c r="G25" s="29">
+        <f t="shared" si="0"/>
+        <v>0.35000000000000003</v>
+      </c>
+      <c r="H25" s="21" t="s">
+        <v>78</v>
+      </c>
+      <c r="I25" s="21"/>
+      <c r="J25" s="15" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="26" spans="2:10" ht="15.6">
+      <c r="B26" s="25" t="s">
+        <v>66</v>
+      </c>
+      <c r="C26" s="30">
+        <v>50222</v>
+      </c>
+      <c r="D26" s="25" t="s">
+        <v>67</v>
+      </c>
+      <c r="E26" s="25"/>
+      <c r="F26" s="24">
+        <v>32.5</v>
+      </c>
+      <c r="G26" s="24">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H25" s="23"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="15"/>
-    </row>
-    <row r="26" spans="2:10" ht="15.6">
-      <c r="B26" s="27" t="s">
-        <v>75</v>
-      </c>
-      <c r="C26" s="32">
-        <v>50222</v>
-      </c>
-      <c r="D26" s="27" t="s">
-        <v>76</v>
-      </c>
-      <c r="E26" s="27"/>
-      <c r="F26" s="26">
-        <v>32.5</v>
-      </c>
-      <c r="G26" s="26">
-        <f t="shared" si="0"/>
-        <v>0</v>
-      </c>
-      <c r="H26" s="25"/>
-      <c r="I26" s="27" t="s">
-        <v>78</v>
+      <c r="H26" s="23"/>
+      <c r="I26" s="25" t="s">
+        <v>86</v>
       </c>
       <c r="J26" s="15" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
     </row>
     <row r="27" spans="2:10" ht="15.6">
@@ -1282,18 +1402,18 @@
       <c r="E27" s="12"/>
       <c r="F27" s="13"/>
       <c r="G27" s="13">
-        <f t="shared" si="0"/>
+        <f>E27*F27</f>
         <v>0</v>
       </c>
       <c r="H27" s="12"/>
       <c r="I27" s="17" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="J27" s="12"/>
     </row>
     <row r="28" spans="2:10" ht="15.6">
       <c r="G28" s="13">
-        <f t="shared" si="0"/>
+        <f>E28*F28</f>
         <v>0</v>
       </c>
     </row>
@@ -1323,29 +1443,29 @@
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="2:10" ht="15.6">
-      <c r="B31" s="28" t="s">
-        <v>57</v>
-      </c>
-      <c r="C31" s="28" t="s">
-        <v>58</v>
-      </c>
-      <c r="D31" s="25"/>
-      <c r="E31" s="25"/>
-      <c r="F31" s="26">
-        <v>11.81</v>
+      <c r="B31" s="26" t="s">
+        <v>48</v>
+      </c>
+      <c r="C31" s="26" t="s">
+        <v>49</v>
+      </c>
+      <c r="D31" s="23"/>
+      <c r="E31" s="23"/>
+      <c r="F31" s="24">
+        <v>11.38</v>
       </c>
       <c r="G31" s="13">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" s="27" t="s">
-        <v>73</v>
-      </c>
-      <c r="I31" s="27" t="s">
-        <v>59</v>
-      </c>
-      <c r="J31" s="12" t="s">
-        <v>60</v>
+      <c r="H31" s="25" t="s">
+        <v>64</v>
+      </c>
+      <c r="I31" s="25" t="s">
+        <v>50</v>
+      </c>
+      <c r="J31" s="15" t="s">
+        <v>51</v>
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.6">
@@ -1357,18 +1477,18 @@
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12">
-        <v>1</v>
+        <v>10</v>
       </c>
       <c r="F32" s="13">
-        <v>0.25</v>
+        <v>0.17</v>
       </c>
       <c r="G32" s="13">
         <f>E32*F32</f>
-        <v>0.25</v>
+        <v>1.7000000000000002</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="14"/>
-      <c r="J32" s="12" t="s">
+      <c r="I32" s="33"/>
+      <c r="J32" s="15" t="s">
         <v>18</v>
       </c>
     </row>
@@ -1381,220 +1501,272 @@
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="F33" s="13">
-        <v>0.41</v>
+        <v>0.39</v>
       </c>
       <c r="G33" s="13">
         <f t="shared" si="0"/>
-        <v>0.41</v>
+        <v>1.17</v>
       </c>
       <c r="H33" s="17" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="I33" s="17"/>
-      <c r="J33" s="12" t="s">
+      <c r="J33" s="15" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="34" spans="2:10" ht="15.6">
-      <c r="B34" s="28" t="s">
+      <c r="B34" s="26" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="28" t="s">
+      <c r="C34" s="26" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="27"/>
-      <c r="E34" s="27">
-        <v>1</v>
-      </c>
-      <c r="F34" s="29">
-        <v>3.07</v>
-      </c>
-      <c r="G34" s="29">
-        <f t="shared" si="0"/>
-        <v>3.07</v>
-      </c>
-      <c r="H34" s="27" t="s">
+      <c r="D34" s="25"/>
+      <c r="E34" s="25"/>
+      <c r="F34" s="27">
+        <v>2.96</v>
+      </c>
+      <c r="G34" s="27">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H34" s="25" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="27"/>
-      <c r="J34" s="17" t="s">
+      <c r="I34" s="25"/>
+      <c r="J34" s="15" t="s">
         <v>22</v>
       </c>
     </row>
     <row r="35" spans="2:10" ht="15.6">
-      <c r="B35" s="22" t="s">
+      <c r="B35" s="20" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="22" t="s">
+      <c r="C35" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="23"/>
-      <c r="E35" s="23">
-        <v>1</v>
-      </c>
-      <c r="F35" s="24">
-        <v>0.47</v>
-      </c>
-      <c r="G35" s="24">
-        <f t="shared" si="0"/>
-        <v>0.47</v>
-      </c>
-      <c r="H35" s="23" t="s">
-        <v>74</v>
-      </c>
-      <c r="I35" s="23"/>
-      <c r="J35" s="17" t="s">
+      <c r="D35" s="21"/>
+      <c r="E35" s="21">
+        <v>10</v>
+      </c>
+      <c r="F35" s="22">
+        <v>0.377</v>
+      </c>
+      <c r="G35" s="22">
+        <f t="shared" si="0"/>
+        <v>3.77</v>
+      </c>
+      <c r="H35" s="21" t="s">
+        <v>65</v>
+      </c>
+      <c r="I35" s="21"/>
+      <c r="J35" s="15" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="36" spans="2:10" ht="15.6">
+      <c r="B36" s="21" t="s">
+        <v>38</v>
+      </c>
+      <c r="C36" s="21" t="s">
+        <v>39</v>
+      </c>
+      <c r="D36" s="21"/>
+      <c r="E36" s="21">
+        <v>10</v>
+      </c>
+      <c r="F36" s="22">
+        <v>0.29099999999999998</v>
+      </c>
+      <c r="G36" s="22">
+        <f t="shared" si="0"/>
+        <v>2.9099999999999997</v>
+      </c>
+      <c r="H36" s="21"/>
+      <c r="I36" s="21"/>
+      <c r="J36" s="15" t="s">
         <v>40</v>
-      </c>
-    </row>
-    <row r="36" spans="2:10" ht="15.6">
-      <c r="B36" s="23" t="s">
-        <v>41</v>
-      </c>
-      <c r="C36" s="23" t="s">
-        <v>42</v>
-      </c>
-      <c r="D36" s="23"/>
-      <c r="E36" s="23">
-        <v>10</v>
-      </c>
-      <c r="F36" s="24">
-        <v>0.20499999999999999</v>
-      </c>
-      <c r="G36" s="24">
-        <f t="shared" si="0"/>
-        <v>2.0499999999999998</v>
-      </c>
-      <c r="H36" s="23"/>
-      <c r="I36" s="23"/>
-      <c r="J36" s="17" t="s">
-        <v>43</v>
       </c>
     </row>
     <row r="37" spans="2:10" ht="15.6">
       <c r="B37" s="17" t="s">
-        <v>36</v>
+        <v>90</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>37</v>
+        <v>89</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17">
         <v>2</v>
       </c>
-      <c r="F37" s="21">
-        <v>1.06</v>
-      </c>
-      <c r="G37" s="21">
-        <f t="shared" si="0"/>
-        <v>2.12</v>
+      <c r="F37" s="19">
+        <v>1.29</v>
+      </c>
+      <c r="G37" s="19">
+        <f t="shared" si="0"/>
+        <v>2.58</v>
       </c>
       <c r="H37" s="17" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="I37" s="17"/>
-      <c r="J37" s="17" t="s">
-        <v>39</v>
+      <c r="J37" s="15" t="s">
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.6">
       <c r="B38" s="12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="C38" s="12" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="D38" s="12"/>
       <c r="E38" s="12">
         <v>1</v>
       </c>
       <c r="F38" s="13">
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
       <c r="G38" s="13">
         <f t="shared" si="0"/>
-        <v>1.38</v>
+        <v>1.33</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>46</v>
+        <v>87</v>
       </c>
       <c r="I38" s="12"/>
-      <c r="J38" s="12" t="s">
-        <v>47</v>
+      <c r="J38" s="15" t="s">
+        <v>43</v>
       </c>
     </row>
     <row r="39" spans="2:10" ht="15.6">
-      <c r="B39" s="12" t="s">
-        <v>50</v>
-      </c>
-      <c r="C39" s="12">
-        <v>483930003</v>
-      </c>
-      <c r="D39" s="12"/>
-      <c r="E39" s="12">
+      <c r="B39" s="25" t="s">
+        <v>99</v>
+      </c>
+      <c r="C39" s="23"/>
+      <c r="D39" s="23"/>
+      <c r="E39" s="23"/>
+      <c r="F39" s="24"/>
+      <c r="G39" s="24">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+      <c r="H39" s="25"/>
+      <c r="I39" s="25" t="s">
+        <v>100</v>
+      </c>
+      <c r="J39" s="12"/>
+    </row>
+    <row r="40" spans="2:10" ht="17.399999999999999">
+      <c r="B40" s="32" t="s">
+        <v>80</v>
+      </c>
+      <c r="C40" s="32" t="s">
+        <v>81</v>
+      </c>
+      <c r="D40" s="17" t="s">
+        <v>82</v>
+      </c>
+      <c r="E40" s="12">
         <v>1</v>
       </c>
-      <c r="F39" s="13">
-        <v>2.56</v>
-      </c>
-      <c r="G39" s="13">
-        <f t="shared" si="0"/>
-        <v>2.56</v>
-      </c>
-      <c r="H39" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="I39" s="12"/>
-      <c r="J39" s="12" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="40" spans="2:10" ht="15.6">
-      <c r="B40" s="12"/>
-      <c r="C40" s="12"/>
-      <c r="D40" s="12"/>
-      <c r="E40" s="12"/>
-      <c r="F40" s="13"/>
-      <c r="G40" s="13"/>
-      <c r="H40" s="12"/>
+      <c r="F40" s="13">
+        <v>20.88</v>
+      </c>
+      <c r="G40" s="13">
+        <f t="shared" si="0"/>
+        <v>20.88</v>
+      </c>
+      <c r="H40" s="17" t="s">
+        <v>83</v>
+      </c>
       <c r="I40" s="12"/>
-      <c r="J40" s="12"/>
+      <c r="J40" s="15" t="s">
+        <v>84</v>
+      </c>
     </row>
     <row r="41" spans="2:10" ht="15.6">
-      <c r="B41" s="12"/>
-      <c r="C41" s="12"/>
+      <c r="B41" s="12" t="s">
+        <v>92</v>
+      </c>
+      <c r="C41" s="12">
+        <v>61300911121</v>
+      </c>
       <c r="D41" s="12"/>
-      <c r="E41" s="12"/>
-      <c r="F41" s="13"/>
-      <c r="G41" s="13"/>
-      <c r="H41" s="12"/>
+      <c r="E41" s="12">
+        <v>2</v>
+      </c>
+      <c r="F41" s="13">
+        <v>0.57999999999999996</v>
+      </c>
+      <c r="G41" s="13">
+        <f t="shared" si="0"/>
+        <v>1.1599999999999999</v>
+      </c>
+      <c r="H41" s="17" t="s">
+        <v>93</v>
+      </c>
       <c r="I41" s="12"/>
-      <c r="J41" s="12"/>
+      <c r="J41" s="15" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="42" spans="2:10" ht="15.6">
-      <c r="B42" s="12"/>
-      <c r="C42" s="12"/>
+      <c r="B42" s="12" t="s">
+        <v>96</v>
+      </c>
+      <c r="C42" s="12" t="s">
+        <v>97</v>
+      </c>
       <c r="D42" s="12"/>
-      <c r="E42" s="12"/>
-      <c r="F42" s="13"/>
-      <c r="G42" s="13"/>
-      <c r="H42" s="12"/>
+      <c r="E42" s="12">
+        <v>2</v>
+      </c>
+      <c r="F42" s="13">
+        <v>1.01</v>
+      </c>
+      <c r="G42" s="13">
+        <f t="shared" si="0"/>
+        <v>2.02</v>
+      </c>
+      <c r="H42" s="17" t="s">
+        <v>94</v>
+      </c>
       <c r="I42" s="12"/>
-      <c r="J42" s="12"/>
+      <c r="J42" s="15" t="s">
+        <v>98</v>
+      </c>
     </row>
     <row r="43" spans="2:10" ht="15.6">
-      <c r="B43" s="12"/>
-      <c r="C43" s="12"/>
+      <c r="B43" s="12" t="s">
+        <v>101</v>
+      </c>
+      <c r="C43" s="12" t="s">
+        <v>102</v>
+      </c>
       <c r="D43" s="12"/>
-      <c r="E43" s="12"/>
-      <c r="F43" s="13"/>
-      <c r="G43" s="13"/>
-      <c r="H43" s="12"/>
+      <c r="E43" s="12">
+        <v>3</v>
+      </c>
+      <c r="F43" s="13">
+        <v>0.47</v>
+      </c>
+      <c r="G43" s="13">
+        <f t="shared" si="0"/>
+        <v>1.41</v>
+      </c>
+      <c r="H43" s="17" t="s">
+        <v>103</v>
+      </c>
       <c r="I43" s="12"/>
-      <c r="J43" s="12"/>
+      <c r="J43" s="12" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="44" spans="2:10" ht="15.6">
       <c r="B44" s="12"/>
@@ -1734,8 +1906,28 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J22" r:id="rId1" xr:uid="{A4DFB0ED-48AD-4D6C-B4E6-A978380DFACD}"/>
+    <hyperlink ref="J26" r:id="rId2" xr:uid="{5869FA7C-E4C3-4F14-98FE-BC512506C711}"/>
+    <hyperlink ref="J33" r:id="rId3" xr:uid="{B0F68EC1-0234-464B-9B44-8F3786E8C5A9}"/>
+    <hyperlink ref="J16" r:id="rId4" xr:uid="{245D86E6-5583-4542-BDC6-1A528EA3099A}"/>
+    <hyperlink ref="J37" r:id="rId5" xr:uid="{EA66ECB7-B2E5-4CBB-B675-84976DC3DB43}"/>
+    <hyperlink ref="J13" r:id="rId6" xr:uid="{C6C2F818-EF15-47AD-BB6A-982A3636DB44}"/>
+    <hyperlink ref="J15" r:id="rId7" xr:uid="{7FE64812-1725-4C9B-8688-810B3B128D3B}"/>
+    <hyperlink ref="J24" r:id="rId8" xr:uid="{6B0095BE-9A2C-4316-A27A-D0294E4CD7B3}"/>
+    <hyperlink ref="J32" r:id="rId9" xr:uid="{241880E7-1D08-4B09-B5E8-00C2BCBD478D}"/>
+    <hyperlink ref="J31" r:id="rId10" xr:uid="{D35248E7-E0E7-4AB3-BB3F-0EE719148224}"/>
+    <hyperlink ref="J35" r:id="rId11" xr:uid="{74E0D7E9-55B0-4630-9E1F-B8A957E3B4C3}"/>
+    <hyperlink ref="J34" r:id="rId12" xr:uid="{7368AF19-FEAE-4E5B-BDB3-A72E7349FA2B}"/>
+    <hyperlink ref="J38" r:id="rId13" xr:uid="{A7DA19D2-DEA6-46D1-BD03-D788201ED8A5}"/>
+    <hyperlink ref="J36" r:id="rId14" xr:uid="{971F29BE-1F1A-496A-8281-5E2C0158D627}"/>
+    <hyperlink ref="J40" r:id="rId15" xr:uid="{A70DDCD3-8F9A-4D3A-81E6-7947B534EE78}"/>
+    <hyperlink ref="J12" r:id="rId16" xr:uid="{0EFE5B53-0BA6-42DE-B75E-DB507B397D4A}"/>
+    <hyperlink ref="J14" r:id="rId17" xr:uid="{D28C2927-D306-4182-A843-F5145C70DC6F}"/>
+    <hyperlink ref="J23" r:id="rId18" xr:uid="{796F67B6-DDD0-4F69-B70C-1433ADA31941}"/>
+    <hyperlink ref="J25" r:id="rId19" xr:uid="{1C16A7C6-A03E-4731-A550-29431CBF774A}"/>
+    <hyperlink ref="J42" r:id="rId20" xr:uid="{C60DC024-092C-4392-BBAD-A1F3F30D04ED}"/>
+    <hyperlink ref="J41" r:id="rId21" xr:uid="{1749C1CD-EE37-49B0-A1AD-C1A54C41332A}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" r:id="rId2"/>
+  <pageSetup scale="56" orientation="portrait" r:id="rId22"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
work some more on the layout, had to move gpio for breakout board still need to hook those up and account for board mounting
</commit_message>
<xml_diff>
--- a/BOM/BOM_ArmPowerBoard_V3.xlsx
+++ b/BOM/BOM_ArmPowerBoard_V3.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21126"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55BDBC16-3402-4271-803D-FD716D06CE1B}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B1E863-F007-4F5C-989A-52822E472B40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23040" windowHeight="8988" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
   <si>
     <t>Description</t>
   </si>
@@ -234,15 +234,6 @@
     <t>externla clock</t>
   </si>
   <si>
-    <t>25W Step Down Adjustable Switching Regulator</t>
-  </si>
-  <si>
-    <t>solarbotics</t>
-  </si>
-  <si>
-    <t>https://solarbotics.com/product/50222/</t>
-  </si>
-  <si>
     <t>DIODE ZENER 28V 5W DO214AA</t>
   </si>
   <si>
@@ -261,18 +252,6 @@
     <t>https://www.digikey.ca/product-detail/en/micro-commercial-co/SMBJ5362B-TP/SMBJ5362B-TPMSCT-ND/1636228</t>
   </si>
   <si>
-    <t>15 Ohms ±1% 0.063W, 1/16W Chip Resistor 0402 (1005 Metric) Automotive AEC-Q200, Moisture Resistant Thick Film</t>
-  </si>
-  <si>
-    <t>CRGCQ0402F15R</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/te-connectivity-passive-product/CRGCQ0402F15R/A129605CT-ND/8577437</t>
-  </si>
-  <si>
-    <t>15Ohm for zener Diode</t>
-  </si>
-  <si>
     <t>min 12 Ohm current limiting</t>
   </si>
   <si>
@@ -294,15 +273,9 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>We have unused 2 good ones</t>
-  </si>
-  <si>
     <t>serial port 7 pin</t>
   </si>
   <si>
-    <t>(lots in random minirover stuff)</t>
-  </si>
-  <si>
     <t>PPTC141LFBN-RC</t>
   </si>
   <si>
@@ -352,6 +325,24 @@
   </si>
   <si>
     <t>ArmPowerBoard</t>
+  </si>
+  <si>
+    <t>CAP CER 10UF 16V X5R 0805</t>
+  </si>
+  <si>
+    <t>CL21A106KOQNNNG</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/samsung-electro-mechanics/CL21A106KOQNNNG/1276-6455-1-ND/5958083</t>
+  </si>
+  <si>
+    <t>DC DC CONVERTER 5V 5W</t>
+  </si>
+  <si>
+    <t>V7805-1000</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/cui-inc/V7805-1000/102-1715-ND/1828608</t>
   </si>
 </sst>
 </file>
@@ -362,7 +353,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="17">
+  <fonts count="18">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -467,13 +458,6 @@
       <family val="2"/>
     </font>
     <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FF000000"/>
-      <name val="Verdana"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="14"/>
       <color rgb="FF555555"/>
       <name val="Arial"/>
@@ -486,6 +470,18 @@
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <name val="Verdana"/>
+      <family val="2"/>
     </font>
   </fonts>
   <fills count="6">
@@ -548,7 +544,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -601,22 +597,25 @@
     <xf numFmtId="165" fontId="1" fillId="5" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="16" fontId="6" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -938,7 +937,7 @@
   <dimension ref="B2:J63"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -955,10 +954,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="23.4">
-      <c r="B2" s="34" t="s">
+      <c r="B2" s="33" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="35"/>
+      <c r="C2" s="34"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -975,7 +974,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -984,7 +983,7 @@
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="31">
+      <c r="C5" s="30">
         <v>43498</v>
       </c>
       <c r="D5" s="1"/>
@@ -1002,7 +1001,7 @@
       </c>
       <c r="C7" s="10">
         <f>SUM(G11:G41)</f>
-        <v>296.56</v>
+        <v>307.92</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
@@ -1251,7 +1250,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1295,10 +1294,10 @@
     </row>
     <row r="23" spans="2:10" ht="15.6">
       <c r="B23" s="17" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
       <c r="C23" s="17" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
       <c r="D23" s="12"/>
       <c r="E23" s="12">
@@ -1312,19 +1311,19 @@
         <v>0.96</v>
       </c>
       <c r="H23" s="17" t="s">
-        <v>79</v>
+        <v>72</v>
       </c>
       <c r="I23" s="12"/>
       <c r="J23" s="15" t="s">
-        <v>74</v>
+        <v>71</v>
       </c>
     </row>
     <row r="24" spans="2:10" ht="15.6">
       <c r="B24" s="17" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
       <c r="C24" s="12" t="s">
-        <v>72</v>
+        <v>69</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12">
@@ -1340,81 +1339,77 @@
       <c r="H24" s="12"/>
       <c r="I24" s="17"/>
       <c r="J24" s="15" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.6">
-      <c r="B25" s="28" t="s">
-        <v>75</v>
-      </c>
-      <c r="C25" s="21" t="s">
-        <v>76</v>
-      </c>
+      <c r="B25" s="21"/>
+      <c r="C25" s="21"/>
       <c r="D25" s="28"/>
-      <c r="E25" s="28">
-        <v>10</v>
-      </c>
-      <c r="F25" s="29">
-        <v>3.5000000000000003E-2</v>
-      </c>
-      <c r="G25" s="29">
-        <f t="shared" si="0"/>
-        <v>0.35000000000000003</v>
-      </c>
-      <c r="H25" s="21" t="s">
-        <v>78</v>
-      </c>
+      <c r="E25" s="28"/>
+      <c r="F25" s="29"/>
+      <c r="G25" s="29"/>
+      <c r="H25" s="21"/>
       <c r="I25" s="21"/>
-      <c r="J25" s="15" t="s">
-        <v>77</v>
-      </c>
+      <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" ht="15.6">
-      <c r="B26" s="25" t="s">
-        <v>66</v>
-      </c>
-      <c r="C26" s="30">
-        <v>50222</v>
-      </c>
-      <c r="D26" s="25" t="s">
-        <v>67</v>
-      </c>
-      <c r="E26" s="25"/>
-      <c r="F26" s="24">
-        <v>32.5</v>
-      </c>
-      <c r="G26" s="24">
+      <c r="B26" s="35"/>
+      <c r="C26" s="36"/>
+      <c r="D26" s="35"/>
+      <c r="E26" s="35"/>
+      <c r="F26" s="37"/>
+      <c r="G26" s="29">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="23"/>
-      <c r="I26" s="25" t="s">
-        <v>86</v>
-      </c>
-      <c r="J26" s="15" t="s">
-        <v>68</v>
-      </c>
+      <c r="H26" s="35"/>
+      <c r="I26" s="35"/>
+      <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" ht="15.6">
-      <c r="B27" s="17"/>
-      <c r="C27" s="12"/>
+      <c r="B27" s="17" t="s">
+        <v>100</v>
+      </c>
+      <c r="C27" s="17" t="s">
+        <v>101</v>
+      </c>
       <c r="D27" s="12"/>
-      <c r="E27" s="12"/>
-      <c r="F27" s="13"/>
+      <c r="E27" s="12">
+        <v>1</v>
+      </c>
+      <c r="F27" s="13">
+        <v>9.9700000000000006</v>
+      </c>
       <c r="G27" s="13">
         <f>E27*F27</f>
-        <v>0</v>
+        <v>9.9700000000000006</v>
       </c>
       <c r="H27" s="12"/>
-      <c r="I27" s="17" t="s">
-        <v>88</v>
-      </c>
-      <c r="J27" s="12"/>
+      <c r="I27" s="17"/>
+      <c r="J27" s="15" t="s">
+        <v>102</v>
+      </c>
     </row>
     <row r="28" spans="2:10" ht="15.6">
+      <c r="B28" t="s">
+        <v>97</v>
+      </c>
+      <c r="C28" s="38" t="s">
+        <v>98</v>
+      </c>
+      <c r="E28" s="17">
+        <v>10</v>
+      </c>
+      <c r="F28" s="19">
+        <v>0.17399999999999999</v>
+      </c>
       <c r="G28" s="13">
         <f>E28*F28</f>
-        <v>0</v>
+        <v>1.7399999999999998</v>
+      </c>
+      <c r="J28" t="s">
+        <v>99</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.6">
@@ -1487,7 +1482,7 @@
         <v>1.7000000000000002</v>
       </c>
       <c r="H32" s="14"/>
-      <c r="I32" s="33"/>
+      <c r="I32" s="32"/>
       <c r="J32" s="15" t="s">
         <v>18</v>
       </c>
@@ -1594,10 +1589,10 @@
     </row>
     <row r="37" spans="2:10" ht="15.6">
       <c r="B37" s="17" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="C37" s="17" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="D37" s="17"/>
       <c r="E37" s="17">
@@ -1615,7 +1610,7 @@
       </c>
       <c r="I37" s="17"/>
       <c r="J37" s="15" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="2:10" ht="15.6">
@@ -1637,7 +1632,7 @@
         <v>1.33</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
       <c r="I38" s="12"/>
       <c r="J38" s="15" t="s">
@@ -1646,7 +1641,7 @@
     </row>
     <row r="39" spans="2:10" ht="15.6">
       <c r="B39" s="25" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="C39" s="23"/>
       <c r="D39" s="23"/>
@@ -1658,19 +1653,19 @@
       </c>
       <c r="H39" s="25"/>
       <c r="I39" s="25" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="J39" s="12"/>
     </row>
     <row r="40" spans="2:10" ht="17.399999999999999">
-      <c r="B40" s="32" t="s">
-        <v>80</v>
-      </c>
-      <c r="C40" s="32" t="s">
-        <v>81</v>
+      <c r="B40" s="31" t="s">
+        <v>73</v>
+      </c>
+      <c r="C40" s="31" t="s">
+        <v>74</v>
       </c>
       <c r="D40" s="17" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="E40" s="12">
         <v>1</v>
@@ -1683,16 +1678,16 @@
         <v>20.88</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="15" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
     </row>
     <row r="41" spans="2:10" ht="15.6">
       <c r="B41" s="12" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="C41" s="12">
         <v>61300911121</v>
@@ -1709,19 +1704,19 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="I41" s="12"/>
       <c r="J41" s="15" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
     </row>
     <row r="42" spans="2:10" ht="15.6">
       <c r="B42" s="12" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12">
@@ -1735,19 +1730,19 @@
         <v>2.02</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="I42" s="12"/>
       <c r="J42" s="15" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
     </row>
     <row r="43" spans="2:10" ht="15.6">
       <c r="B43" s="12" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="C43" s="12" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12">
@@ -1761,11 +1756,11 @@
         <v>1.41</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="I43" s="12"/>
       <c r="J43" s="12" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
     </row>
     <row r="44" spans="2:10" ht="15.6">
@@ -1906,28 +1901,27 @@
   </mergeCells>
   <hyperlinks>
     <hyperlink ref="J22" r:id="rId1" xr:uid="{A4DFB0ED-48AD-4D6C-B4E6-A978380DFACD}"/>
-    <hyperlink ref="J26" r:id="rId2" xr:uid="{5869FA7C-E4C3-4F14-98FE-BC512506C711}"/>
-    <hyperlink ref="J33" r:id="rId3" xr:uid="{B0F68EC1-0234-464B-9B44-8F3786E8C5A9}"/>
-    <hyperlink ref="J16" r:id="rId4" xr:uid="{245D86E6-5583-4542-BDC6-1A528EA3099A}"/>
-    <hyperlink ref="J37" r:id="rId5" xr:uid="{EA66ECB7-B2E5-4CBB-B675-84976DC3DB43}"/>
-    <hyperlink ref="J13" r:id="rId6" xr:uid="{C6C2F818-EF15-47AD-BB6A-982A3636DB44}"/>
-    <hyperlink ref="J15" r:id="rId7" xr:uid="{7FE64812-1725-4C9B-8688-810B3B128D3B}"/>
-    <hyperlink ref="J24" r:id="rId8" xr:uid="{6B0095BE-9A2C-4316-A27A-D0294E4CD7B3}"/>
-    <hyperlink ref="J32" r:id="rId9" xr:uid="{241880E7-1D08-4B09-B5E8-00C2BCBD478D}"/>
-    <hyperlink ref="J31" r:id="rId10" xr:uid="{D35248E7-E0E7-4AB3-BB3F-0EE719148224}"/>
-    <hyperlink ref="J35" r:id="rId11" xr:uid="{74E0D7E9-55B0-4630-9E1F-B8A957E3B4C3}"/>
-    <hyperlink ref="J34" r:id="rId12" xr:uid="{7368AF19-FEAE-4E5B-BDB3-A72E7349FA2B}"/>
-    <hyperlink ref="J38" r:id="rId13" xr:uid="{A7DA19D2-DEA6-46D1-BD03-D788201ED8A5}"/>
-    <hyperlink ref="J36" r:id="rId14" xr:uid="{971F29BE-1F1A-496A-8281-5E2C0158D627}"/>
-    <hyperlink ref="J40" r:id="rId15" xr:uid="{A70DDCD3-8F9A-4D3A-81E6-7947B534EE78}"/>
-    <hyperlink ref="J12" r:id="rId16" xr:uid="{0EFE5B53-0BA6-42DE-B75E-DB507B397D4A}"/>
-    <hyperlink ref="J14" r:id="rId17" xr:uid="{D28C2927-D306-4182-A843-F5145C70DC6F}"/>
-    <hyperlink ref="J23" r:id="rId18" xr:uid="{796F67B6-DDD0-4F69-B70C-1433ADA31941}"/>
-    <hyperlink ref="J25" r:id="rId19" xr:uid="{1C16A7C6-A03E-4731-A550-29431CBF774A}"/>
-    <hyperlink ref="J42" r:id="rId20" xr:uid="{C60DC024-092C-4392-BBAD-A1F3F30D04ED}"/>
-    <hyperlink ref="J41" r:id="rId21" xr:uid="{1749C1CD-EE37-49B0-A1AD-C1A54C41332A}"/>
+    <hyperlink ref="J33" r:id="rId2" xr:uid="{B0F68EC1-0234-464B-9B44-8F3786E8C5A9}"/>
+    <hyperlink ref="J16" r:id="rId3" xr:uid="{245D86E6-5583-4542-BDC6-1A528EA3099A}"/>
+    <hyperlink ref="J37" r:id="rId4" xr:uid="{EA66ECB7-B2E5-4CBB-B675-84976DC3DB43}"/>
+    <hyperlink ref="J13" r:id="rId5" xr:uid="{C6C2F818-EF15-47AD-BB6A-982A3636DB44}"/>
+    <hyperlink ref="J15" r:id="rId6" xr:uid="{7FE64812-1725-4C9B-8688-810B3B128D3B}"/>
+    <hyperlink ref="J24" r:id="rId7" xr:uid="{6B0095BE-9A2C-4316-A27A-D0294E4CD7B3}"/>
+    <hyperlink ref="J32" r:id="rId8" xr:uid="{241880E7-1D08-4B09-B5E8-00C2BCBD478D}"/>
+    <hyperlink ref="J31" r:id="rId9" xr:uid="{D35248E7-E0E7-4AB3-BB3F-0EE719148224}"/>
+    <hyperlink ref="J35" r:id="rId10" xr:uid="{74E0D7E9-55B0-4630-9E1F-B8A957E3B4C3}"/>
+    <hyperlink ref="J34" r:id="rId11" xr:uid="{7368AF19-FEAE-4E5B-BDB3-A72E7349FA2B}"/>
+    <hyperlink ref="J38" r:id="rId12" xr:uid="{A7DA19D2-DEA6-46D1-BD03-D788201ED8A5}"/>
+    <hyperlink ref="J36" r:id="rId13" xr:uid="{971F29BE-1F1A-496A-8281-5E2C0158D627}"/>
+    <hyperlink ref="J40" r:id="rId14" xr:uid="{A70DDCD3-8F9A-4D3A-81E6-7947B534EE78}"/>
+    <hyperlink ref="J12" r:id="rId15" xr:uid="{0EFE5B53-0BA6-42DE-B75E-DB507B397D4A}"/>
+    <hyperlink ref="J14" r:id="rId16" xr:uid="{D28C2927-D306-4182-A843-F5145C70DC6F}"/>
+    <hyperlink ref="J23" r:id="rId17" xr:uid="{796F67B6-DDD0-4F69-B70C-1433ADA31941}"/>
+    <hyperlink ref="J42" r:id="rId18" xr:uid="{C60DC024-092C-4392-BBAD-A1F3F30D04ED}"/>
+    <hyperlink ref="J41" r:id="rId19" xr:uid="{1749C1CD-EE37-49B0-A1AD-C1A54C41332A}"/>
+    <hyperlink ref="J27" r:id="rId20" xr:uid="{87C57A5D-7B3D-438F-A607-45ED8D90C683}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="56" orientation="portrait" r:id="rId22"/>
+  <pageSetup scale="56" orientation="portrait" r:id="rId21"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
updated bom with correct headers
</commit_message>
<xml_diff>
--- a/BOM/BOM_ArmPowerBoard_V3.xlsx
+++ b/BOM/BOM_ArmPowerBoard_V3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\riley\USST\rover-hardware\BOM\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09B1E863-F007-4F5C-989A-52822E472B40}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{157DC3F8-2B33-4300-8787-6558E7505752}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{707F39ED-FB34-4E84-8EC1-DB542E47F720}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="104" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="102">
   <si>
     <t>Description</t>
   </si>
@@ -252,9 +252,6 @@
     <t>https://www.digikey.ca/product-detail/en/micro-commercial-co/SMBJ5362B-TP/SMBJ5362B-TPMSCT-ND/1636228</t>
   </si>
   <si>
-    <t>min 12 Ohm current limiting</t>
-  </si>
-  <si>
     <t>SparkFun USB to Serial Breakout </t>
   </si>
   <si>
@@ -276,15 +273,6 @@
     <t>serial port 7 pin</t>
   </si>
   <si>
-    <t>PPTC141LFBN-RC</t>
-  </si>
-  <si>
-    <t>CONN HDR 14POS 0.1 TIN PCB</t>
-  </si>
-  <si>
-    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPTC141LFBN-RC/S7012-ND/810152</t>
-  </si>
-  <si>
     <t>CONN HEADER VERT 9POS 2.54MM</t>
   </si>
   <si>
@@ -343,6 +331,15 @@
   </si>
   <si>
     <t>https://www.digikey.ca/product-detail/en/cui-inc/V7805-1000/102-1715-ND/1828608</t>
+  </si>
+  <si>
+    <t>CONN HDR 20POS 0.1 GOLD PCB</t>
+  </si>
+  <si>
+    <t>PPPC102LFBN-RC</t>
+  </si>
+  <si>
+    <t>https://www.digikey.ca/product-detail/en/sullins-connector-solutions/PPPC102LFBN-RC/S6106-ND/807245</t>
   </si>
 </sst>
 </file>
@@ -353,7 +350,7 @@
     <numFmt numFmtId="164" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
     <numFmt numFmtId="165" formatCode="&quot;$&quot;#,##0.00"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="19">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -483,8 +480,15 @@
       <name val="Verdana"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -515,6 +519,11 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="2">
     <border>
@@ -540,11 +549,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -586,7 +596,6 @@
     <xf numFmtId="0" fontId="12" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="165" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
@@ -603,21 +612,27 @@
     <xf numFmtId="0" fontId="14" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="165" fontId="16" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="0" xfId="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="10" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="15" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="18" fillId="6" borderId="0" xfId="2"/>
+    <xf numFmtId="165" fontId="18" fillId="6" borderId="0" xfId="2" applyNumberFormat="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
@@ -934,10 +949,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="B2:J63"/>
+  <dimension ref="B2:K63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="D29" sqref="D29"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="75" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="B41" sqref="B41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.77734375" defaultRowHeight="14.4"/>
@@ -954,10 +969,10 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:10" ht="23.4">
-      <c r="B2" s="33" t="s">
+      <c r="B2" s="34" t="s">
         <v>13</v>
       </c>
-      <c r="C2" s="34"/>
+      <c r="C2" s="35"/>
       <c r="D2" s="1"/>
       <c r="E2" s="1"/>
     </row>
@@ -974,7 +989,7 @@
         <v>10</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="D4" s="1"/>
       <c r="E4" s="1"/>
@@ -983,7 +998,7 @@
       <c r="B5" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="30">
+      <c r="C5" s="29">
         <v>43498</v>
       </c>
       <c r="D5" s="1"/>
@@ -1001,7 +1016,7 @@
       </c>
       <c r="C7" s="10">
         <f>SUM(G11:G41)</f>
-        <v>307.92</v>
+        <v>307.13000000000005</v>
       </c>
       <c r="D7" s="1"/>
       <c r="E7" s="5"/>
@@ -1250,7 +1265,7 @@
         <v>0</v>
       </c>
       <c r="H20" s="17" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="I20" s="12"/>
       <c r="J20" s="12"/>
@@ -1310,9 +1325,7 @@
         <f t="shared" si="0"/>
         <v>0.96</v>
       </c>
-      <c r="H23" s="17" t="s">
-        <v>72</v>
-      </c>
+      <c r="H23" s="17"/>
       <c r="I23" s="12"/>
       <c r="J23" s="15" t="s">
         <v>71</v>
@@ -1343,36 +1356,36 @@
       </c>
     </row>
     <row r="25" spans="2:10" ht="15.6">
-      <c r="B25" s="21"/>
-      <c r="C25" s="21"/>
-      <c r="D25" s="28"/>
-      <c r="E25" s="28"/>
-      <c r="F25" s="29"/>
-      <c r="G25" s="29"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="21"/>
+      <c r="B25" s="20"/>
+      <c r="C25" s="20"/>
+      <c r="D25" s="27"/>
+      <c r="E25" s="27"/>
+      <c r="F25" s="28"/>
+      <c r="G25" s="28"/>
+      <c r="H25" s="20"/>
+      <c r="I25" s="20"/>
       <c r="J25" s="15"/>
     </row>
     <row r="26" spans="2:10" ht="15.6">
-      <c r="B26" s="35"/>
-      <c r="C26" s="36"/>
-      <c r="D26" s="35"/>
-      <c r="E26" s="35"/>
-      <c r="F26" s="37"/>
-      <c r="G26" s="29">
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
+      <c r="D26" s="31"/>
+      <c r="E26" s="31"/>
+      <c r="F26" s="33"/>
+      <c r="G26" s="28">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H26" s="35"/>
-      <c r="I26" s="35"/>
+      <c r="H26" s="31"/>
+      <c r="I26" s="31"/>
       <c r="J26" s="15"/>
     </row>
     <row r="27" spans="2:10" ht="15.6">
       <c r="B27" s="17" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="C27" s="17" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="D27" s="12"/>
       <c r="E27" s="12">
@@ -1388,28 +1401,31 @@
       <c r="H27" s="12"/>
       <c r="I27" s="17"/>
       <c r="J27" s="15" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
     </row>
     <row r="28" spans="2:10" ht="15.6">
-      <c r="B28" t="s">
-        <v>97</v>
-      </c>
-      <c r="C28" s="38" t="s">
-        <v>98</v>
-      </c>
-      <c r="E28" s="17">
+      <c r="B28" s="37" t="s">
+        <v>93</v>
+      </c>
+      <c r="C28" s="40" t="s">
+        <v>94</v>
+      </c>
+      <c r="D28" s="37"/>
+      <c r="E28" s="24">
         <v>10</v>
       </c>
-      <c r="F28" s="19">
+      <c r="F28" s="26">
         <v>0.17399999999999999</v>
       </c>
-      <c r="G28" s="13">
+      <c r="G28" s="23">
         <f>E28*F28</f>
         <v>1.7399999999999998</v>
       </c>
+      <c r="H28" s="37"/>
+      <c r="I28" s="37"/>
       <c r="J28" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
     </row>
     <row r="29" spans="2:10" ht="15.6">
@@ -1438,25 +1454,25 @@
       <c r="J30" s="12"/>
     </row>
     <row r="31" spans="2:10" ht="15.6">
-      <c r="B31" s="26" t="s">
+      <c r="B31" s="25" t="s">
         <v>48</v>
       </c>
-      <c r="C31" s="26" t="s">
+      <c r="C31" s="25" t="s">
         <v>49</v>
       </c>
-      <c r="D31" s="23"/>
-      <c r="E31" s="23"/>
-      <c r="F31" s="24">
+      <c r="D31" s="22"/>
+      <c r="E31" s="22"/>
+      <c r="F31" s="23">
         <v>11.38</v>
       </c>
-      <c r="G31" s="13">
+      <c r="G31" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H31" s="25" t="s">
+      <c r="H31" s="24" t="s">
         <v>64</v>
       </c>
-      <c r="I31" s="25" t="s">
+      <c r="I31" s="24" t="s">
         <v>50</v>
       </c>
       <c r="J31" s="15" t="s">
@@ -1464,30 +1480,30 @@
       </c>
     </row>
     <row r="32" spans="2:10" ht="15.6">
-      <c r="B32" s="17" t="s">
+      <c r="B32" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="C32" s="12" t="s">
+      <c r="C32" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="D32" s="12"/>
-      <c r="E32" s="12">
+      <c r="D32" s="22"/>
+      <c r="E32" s="22">
         <v>10</v>
       </c>
-      <c r="F32" s="13">
+      <c r="F32" s="23">
         <v>0.17</v>
       </c>
-      <c r="G32" s="13">
+      <c r="G32" s="23">
         <f>E32*F32</f>
         <v>1.7000000000000002</v>
       </c>
-      <c r="H32" s="14"/>
-      <c r="I32" s="32"/>
+      <c r="H32" s="38"/>
+      <c r="I32" s="39"/>
       <c r="J32" s="15" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="33" spans="2:10" ht="15.6">
+    <row r="33" spans="2:11" ht="15.6">
       <c r="B33" s="17" t="s">
         <v>32</v>
       </c>
@@ -1513,107 +1529,108 @@
         <v>34</v>
       </c>
     </row>
-    <row r="34" spans="2:10" ht="15.6">
-      <c r="B34" s="26" t="s">
+    <row r="34" spans="2:11" ht="15.6">
+      <c r="B34" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="C34" s="26" t="s">
+      <c r="C34" s="25" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="25"/>
-      <c r="E34" s="25"/>
-      <c r="F34" s="27">
+      <c r="D34" s="24"/>
+      <c r="E34" s="24"/>
+      <c r="F34" s="26">
         <v>2.96</v>
       </c>
-      <c r="G34" s="27">
+      <c r="G34" s="26">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H34" s="25" t="s">
+      <c r="H34" s="24" t="s">
         <v>35</v>
       </c>
-      <c r="I34" s="25"/>
+      <c r="I34" s="24"/>
       <c r="J34" s="15" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="35" spans="2:10" ht="15.6">
-      <c r="B35" s="20" t="s">
+    <row r="35" spans="2:11" ht="15.6">
+      <c r="B35" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="C35" s="20" t="s">
+      <c r="C35" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D35" s="21"/>
-      <c r="E35" s="21">
+      <c r="D35" s="20"/>
+      <c r="E35" s="20">
         <v>10</v>
       </c>
-      <c r="F35" s="22">
+      <c r="F35" s="21">
         <v>0.377</v>
       </c>
-      <c r="G35" s="22">
+      <c r="G35" s="21">
         <f t="shared" si="0"/>
         <v>3.77</v>
       </c>
-      <c r="H35" s="21" t="s">
+      <c r="H35" s="20" t="s">
         <v>65</v>
       </c>
-      <c r="I35" s="21"/>
+      <c r="I35" s="20"/>
       <c r="J35" s="15" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="2:10" ht="15.6">
-      <c r="B36" s="21" t="s">
+    <row r="36" spans="2:11" ht="15.6">
+      <c r="B36" s="24" t="s">
         <v>38</v>
       </c>
-      <c r="C36" s="21" t="s">
+      <c r="C36" s="24" t="s">
         <v>39</v>
       </c>
-      <c r="D36" s="21"/>
-      <c r="E36" s="21">
+      <c r="D36" s="24"/>
+      <c r="E36" s="24">
         <v>10</v>
       </c>
-      <c r="F36" s="22">
+      <c r="F36" s="26">
         <v>0.29099999999999998</v>
       </c>
-      <c r="G36" s="22">
+      <c r="G36" s="26">
         <f t="shared" si="0"/>
         <v>2.9099999999999997</v>
       </c>
-      <c r="H36" s="21"/>
-      <c r="I36" s="21"/>
-      <c r="J36" s="15" t="s">
+      <c r="H36" s="24"/>
+      <c r="I36" s="24"/>
+      <c r="J36" s="36" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="37" spans="2:10" ht="15.6">
-      <c r="B37" s="17" t="s">
-        <v>81</v>
-      </c>
-      <c r="C37" s="17" t="s">
-        <v>80</v>
-      </c>
-      <c r="D37" s="17"/>
-      <c r="E37" s="17">
-        <v>2</v>
-      </c>
-      <c r="F37" s="19">
-        <v>1.29</v>
-      </c>
-      <c r="G37" s="19">
-        <f t="shared" si="0"/>
-        <v>2.58</v>
-      </c>
-      <c r="H37" s="17" t="s">
+      <c r="K36" s="37"/>
+    </row>
+    <row r="37" spans="2:11">
+      <c r="B37" s="41" t="s">
+        <v>99</v>
+      </c>
+      <c r="C37" s="41" t="s">
+        <v>100</v>
+      </c>
+      <c r="D37" s="41"/>
+      <c r="E37" s="41">
+        <v>1</v>
+      </c>
+      <c r="F37" s="42">
+        <v>1.79</v>
+      </c>
+      <c r="G37" s="42">
+        <f t="shared" si="0"/>
+        <v>1.79</v>
+      </c>
+      <c r="H37" s="41" t="s">
         <v>36</v>
       </c>
-      <c r="I37" s="17"/>
-      <c r="J37" s="15" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="38" spans="2:10" ht="15.6">
+      <c r="I37" s="41"/>
+      <c r="J37" s="41" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="38" spans="2:11" ht="15.6">
       <c r="B38" s="12" t="s">
         <v>41</v>
       </c>
@@ -1632,40 +1649,40 @@
         <v>1.33</v>
       </c>
       <c r="H38" s="17" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="I38" s="12"/>
       <c r="J38" s="15" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="39" spans="2:10" ht="15.6">
-      <c r="B39" s="25" t="s">
-        <v>90</v>
-      </c>
-      <c r="C39" s="23"/>
-      <c r="D39" s="23"/>
-      <c r="E39" s="23"/>
-      <c r="F39" s="24"/>
-      <c r="G39" s="24">
+    <row r="39" spans="2:11" ht="15.6">
+      <c r="B39" s="24" t="s">
+        <v>86</v>
+      </c>
+      <c r="C39" s="22"/>
+      <c r="D39" s="22"/>
+      <c r="E39" s="22"/>
+      <c r="F39" s="23"/>
+      <c r="G39" s="23">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
-      <c r="H39" s="25"/>
-      <c r="I39" s="25" t="s">
-        <v>91</v>
+      <c r="H39" s="24"/>
+      <c r="I39" s="24" t="s">
+        <v>87</v>
       </c>
       <c r="J39" s="12"/>
     </row>
-    <row r="40" spans="2:10" ht="17.399999999999999">
-      <c r="B40" s="31" t="s">
+    <row r="40" spans="2:11" ht="17.399999999999999">
+      <c r="B40" s="30" t="s">
+        <v>72</v>
+      </c>
+      <c r="C40" s="30" t="s">
         <v>73</v>
       </c>
-      <c r="C40" s="31" t="s">
+      <c r="D40" s="17" t="s">
         <v>74</v>
-      </c>
-      <c r="D40" s="17" t="s">
-        <v>75</v>
       </c>
       <c r="E40" s="12">
         <v>1</v>
@@ -1678,16 +1695,16 @@
         <v>20.88</v>
       </c>
       <c r="H40" s="17" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="I40" s="12"/>
       <c r="J40" s="15" t="s">
-        <v>77</v>
-      </c>
-    </row>
-    <row r="41" spans="2:10" ht="15.6">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="41" spans="2:11" ht="15.6">
       <c r="B41" s="12" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="C41" s="12">
         <v>61300911121</v>
@@ -1704,19 +1721,19 @@
         <v>1.1599999999999999</v>
       </c>
       <c r="H41" s="17" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="I41" s="12"/>
       <c r="J41" s="15" t="s">
-        <v>86</v>
-      </c>
-    </row>
-    <row r="42" spans="2:10" ht="15.6">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="2:11" ht="15.6">
       <c r="B42" s="12" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="C42" s="12" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12">
@@ -1730,19 +1747,19 @@
         <v>2.02</v>
       </c>
       <c r="H42" s="17" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="I42" s="12"/>
       <c r="J42" s="15" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="43" spans="2:11" ht="15.6">
+      <c r="B43" s="12" t="s">
+        <v>88</v>
+      </c>
+      <c r="C43" s="12" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="43" spans="2:10" ht="15.6">
-      <c r="B43" s="12" t="s">
-        <v>92</v>
-      </c>
-      <c r="C43" s="12" t="s">
-        <v>93</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12">
@@ -1756,14 +1773,14 @@
         <v>1.41</v>
       </c>
       <c r="H43" s="17" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="I43" s="12"/>
       <c r="J43" s="12" t="s">
-        <v>95</v>
-      </c>
-    </row>
-    <row r="44" spans="2:10" ht="15.6">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="44" spans="2:11" ht="15.6">
       <c r="B44" s="12"/>
       <c r="C44" s="12"/>
       <c r="D44" s="12"/>
@@ -1774,7 +1791,7 @@
       <c r="I44" s="12"/>
       <c r="J44" s="12"/>
     </row>
-    <row r="45" spans="2:10" ht="15.6">
+    <row r="45" spans="2:11" ht="15.6">
       <c r="B45" s="12"/>
       <c r="C45" s="12"/>
       <c r="D45" s="12"/>
@@ -1785,7 +1802,7 @@
       <c r="I45" s="12"/>
       <c r="J45" s="12"/>
     </row>
-    <row r="46" spans="2:10" ht="15.6">
+    <row r="46" spans="2:11" ht="15.6">
       <c r="B46" s="12"/>
       <c r="C46" s="12"/>
       <c r="D46" s="12"/>
@@ -1796,7 +1813,7 @@
       <c r="I46" s="12"/>
       <c r="J46" s="12"/>
     </row>
-    <row r="47" spans="2:10" ht="15.6">
+    <row r="47" spans="2:11" ht="15.6">
       <c r="B47" s="12"/>
       <c r="C47" s="12"/>
       <c r="D47" s="12"/>
@@ -1807,7 +1824,7 @@
       <c r="I47" s="12"/>
       <c r="J47" s="12"/>
     </row>
-    <row r="48" spans="2:10" ht="15.6">
+    <row r="48" spans="2:11" ht="15.6">
       <c r="B48" s="12"/>
       <c r="C48" s="12"/>
       <c r="D48" s="12"/>

</xml_diff>